<commit_message>
updating power consumption stats
</commit_message>
<xml_diff>
--- a/Results/power_consumption.xlsx
+++ b/Results/power_consumption.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joe/Documents/Research/Embedded_miniHarp/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8344AA-52DC-5546-A6ED-6D4ECB911691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8D48B5-E4D6-3C4C-973A-6EF8BAA388AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{8786ABF1-DC7F-214F-BF56-4D122C35DF65}"/>
+    <workbookView xWindow="-220" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{8786ABF1-DC7F-214F-BF56-4D122C35DF65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Wh</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>prog (only detector, sleep)</t>
+  </si>
+  <si>
+    <t>prog (lots of tapping)</t>
+  </si>
+  <si>
+    <t>Raspberry Pi zero</t>
+  </si>
+  <si>
+    <t>Idel or Program running?</t>
+  </si>
+  <si>
+    <t>Realtime</t>
+  </si>
+  <si>
+    <t>buffer overload</t>
   </si>
 </sst>
 </file>
@@ -437,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC784E1-E55D-DB43-B71D-5A88F5F23FB7}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,19 +463,41 @@
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -470,8 +507,24 @@
       <c r="D5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>0.05</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <f>(K5*3600)/(L5*60 +M5)</f>
+        <v>1.4634146341463414</v>
+      </c>
+      <c r="O5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>0.43509999999999999</v>
       </c>
@@ -488,8 +541,24 @@
       <c r="F6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>0.14380000000000001</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>45</v>
+      </c>
+      <c r="N6">
+        <f>(K6*3600)/(L6*60 +M6)</f>
+        <v>1.8164210526315792</v>
+      </c>
+      <c r="O6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>0.87</v>
       </c>
@@ -506,8 +575,27 @@
       <c r="F7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f>(K7*3600)/(L7*60 +M7)</f>
+        <v>2.0700000000000003</v>
+      </c>
+      <c r="O7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>0.33910000000000001</v>
       </c>
@@ -525,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>0.52129999999999999</v>
       </c>
@@ -543,7 +631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>0.49309999999999998</v>
       </c>
@@ -561,12 +649,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>0.2626</v>
       </c>
@@ -577,14 +665,14 @@
         <v>21</v>
       </c>
       <c r="E14">
-        <f>(B14*3600)/(C14*60 +D14)</f>
+        <f t="shared" ref="E14:E21" si="0">(B14*3600)/(C14*60 +D14)</f>
         <v>1.5223188405797101</v>
       </c>
       <c r="F14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>0.19109999999999999</v>
       </c>
@@ -595,14 +683,14 @@
         <v>36</v>
       </c>
       <c r="E15">
-        <f>(B15*3600)/(C15*60 +D15)</f>
+        <f t="shared" si="0"/>
         <v>1.5086842105263156</v>
       </c>
       <c r="F15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>0.45960000000000001</v>
       </c>
@@ -613,7 +701,7 @@
         <v>18</v>
       </c>
       <c r="E16">
-        <f>(B16*3600)/(C16*60 +D16)</f>
+        <f t="shared" si="0"/>
         <v>2.9651612903225804</v>
       </c>
       <c r="F16" t="s">
@@ -631,7 +719,7 @@
         <v>47</v>
       </c>
       <c r="E17">
-        <f>(B17*3600)/(C17*60 +D17)</f>
+        <f t="shared" si="0"/>
         <v>2.9728222996515679</v>
       </c>
       <c r="F17" t="s">
@@ -649,7 +737,7 @@
         <v>58</v>
       </c>
       <c r="E18">
-        <f>(B18*3600)/(C18*60 +D18)</f>
+        <f t="shared" si="0"/>
         <v>2.9773860182370822</v>
       </c>
       <c r="F18" t="s">
@@ -667,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <f>(B19*3600)/(C19*60 +D19)</f>
+        <f t="shared" si="0"/>
         <v>2.9769999999999999</v>
       </c>
       <c r="F19" t="s">
@@ -685,7 +773,7 @@
         <v>47</v>
       </c>
       <c r="E20">
-        <f>(B20*3600)/(C20*60 +D20)</f>
+        <f t="shared" si="0"/>
         <v>2.2042260442260444</v>
       </c>
       <c r="F20" t="s">
@@ -703,7 +791,7 @@
         <v>15</v>
       </c>
       <c r="E21">
-        <f>(B21*3600)/(C21*60 +D21)</f>
+        <f t="shared" si="0"/>
         <v>2.1983999999999999</v>
       </c>
     </row>

</xml_diff>